<commit_message>
change expected results which were related to the null value transfered to false issue fixed
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/prepareStatement/mysql_ps_batch_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/prepareStatement/mysql_ps_batch_cases.xlsx
@@ -148,19 +148,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select count(*) from $schema26 where id&gt;400 and id&lt;=6000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5600</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>update $schema26 set name='BJ' where id&gt;400 and id&lt;=6000</t>
+    <t>20000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select count(*) from $schema26 where id&gt;4000 and id&lt;=20000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $schema26 set name='BJ' where id&gt;4000 and id&lt;=20000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>